<commit_message>
Fixes Removal of Support Card table
</commit_message>
<xml_diff>
--- a/Uma Run ERD.xlsx
+++ b/Uma Run ERD.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="80">
   <si>
     <t>Player</t>
   </si>
@@ -199,15 +199,27 @@
     <t>Long Sparks</t>
   </si>
   <si>
+    <t>Support Card</t>
+  </si>
+  <si>
     <t>Front Sparks</t>
   </si>
   <si>
+    <t>Support_ID</t>
+  </si>
+  <si>
     <t>Pace Sparks</t>
   </si>
   <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
     <t>Late Sparks</t>
   </si>
   <si>
+    <t>support type</t>
+  </si>
+  <si>
     <t>End Sparks</t>
   </si>
   <si>
@@ -218,6 +230,9 @@
   </si>
   <si>
     <t>default 'G'</t>
+  </si>
+  <si>
+    <t>tinyint</t>
   </si>
   <si>
     <t>Completed</t>
@@ -296,7 +311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +346,12 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor theme="7"/>
       </patternFill>
     </fill>
     <fill>
@@ -390,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -436,13 +457,16 @@
     <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="4" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1497,8 +1521,16 @@
       <c r="M34" s="9"/>
     </row>
     <row r="35">
+      <c r="A35" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="3"/>
       <c r="H35" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I35" s="16" t="s">
         <v>3</v>
@@ -1513,8 +1545,26 @@
       <c r="M35" s="9"/>
     </row>
     <row r="36">
+      <c r="A36" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>7</v>
+      </c>
       <c r="H36" s="16" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I36" s="16" t="s">
         <v>3</v>
@@ -1529,8 +1579,20 @@
       <c r="M36" s="9"/>
     </row>
     <row r="37">
+      <c r="A37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
       <c r="H37" s="16" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="I37" s="16" t="s">
         <v>3</v>
@@ -1545,8 +1607,20 @@
       <c r="M37" s="9"/>
     </row>
     <row r="38">
+      <c r="A38" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
       <c r="H38" s="16" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I38" s="16" t="s">
         <v>3</v>
@@ -1561,46 +1635,74 @@
       <c r="M38" s="9"/>
     </row>
     <row r="39">
+      <c r="A39" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
       <c r="H39" s="16" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>4</v>
       </c>
       <c r="K39" s="16" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="9"/>
     </row>
     <row r="40">
+      <c r="A40" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
       <c r="H40" s="16" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="J40" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="K40" s="17" t="b">
+        <v>76</v>
+      </c>
+      <c r="K40" s="18" t="b">
         <v>0</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
     </row>
     <row r="41">
-      <c r="H41" s="18"/>
-      <c r="I41" s="18"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
+      <c r="H41" s="19"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
     </row>
     <row r="42">
-      <c r="H42" s="19" t="s">
-        <v>72</v>
+      <c r="H42" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2"/>
@@ -1608,7 +1710,7 @@
     </row>
     <row r="43">
       <c r="H43" s="5" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>3</v>
@@ -1616,13 +1718,13 @@
       <c r="J43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="20" t="s">
+      <c r="K43" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44">
       <c r="H44" s="5" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>3</v>
@@ -1635,12 +1737,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H42:K42"/>
     <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A35:F35"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixes Removal of Skills table
</commit_message>
<xml_diff>
--- a/Uma Run ERD.xlsx
+++ b/Uma Run ERD.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="82">
   <si>
     <t>Player</t>
   </si>
@@ -94,24 +94,24 @@
     <t>varchar(1)</t>
   </si>
   <si>
+    <t>Sprint Apt</t>
+  </si>
+  <si>
+    <t>Dirt Apt</t>
+  </si>
+  <si>
+    <t>Mile Apt</t>
+  </si>
+  <si>
     <t>Medium Apt</t>
   </si>
   <si>
-    <t>Dirt Apt</t>
-  </si>
-  <si>
     <t>Long Apt</t>
   </si>
   <si>
-    <t>Sprint Apt</t>
-  </si>
-  <si>
     <t>Front Apt</t>
   </si>
   <si>
-    <t>Mile Apt</t>
-  </si>
-  <si>
     <t>Pace Apt</t>
   </si>
   <si>
@@ -121,12 +121,117 @@
     <t>End Apt</t>
   </si>
   <si>
-    <t>Type</t>
+    <t>Potential</t>
+  </si>
+  <si>
+    <t>tinyint</t>
+  </si>
+  <si>
+    <t>Speed Sparks</t>
+  </si>
+  <si>
+    <t>default 0</t>
+  </si>
+  <si>
+    <t>Stamina Sparks</t>
+  </si>
+  <si>
+    <t>Power Sparks</t>
+  </si>
+  <si>
+    <t>Deck</t>
+  </si>
+  <si>
+    <t>Guts Sparks</t>
+  </si>
+  <si>
+    <t>Wit Sparks</t>
+  </si>
+  <si>
+    <t>Support 1</t>
+  </si>
+  <si>
+    <t>Turf Sparks</t>
+  </si>
+  <si>
+    <t>Support 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">int </t>
+  </si>
+  <si>
+    <t>Dirt Sparks</t>
+  </si>
+  <si>
+    <t>Support 3</t>
+  </si>
+  <si>
+    <t>Sprint Sparks</t>
+  </si>
+  <si>
+    <t>Support 4</t>
+  </si>
+  <si>
+    <t>Mile Sparks</t>
+  </si>
+  <si>
+    <t>Support 5</t>
+  </si>
+  <si>
+    <t>Medium Sparks</t>
+  </si>
+  <si>
+    <t>Support 6</t>
+  </si>
+  <si>
+    <t>Long Sparks</t>
+  </si>
+  <si>
+    <t>Front Sparks</t>
+  </si>
+  <si>
+    <t>Pace Sparks</t>
+  </si>
+  <si>
+    <t>Support Card</t>
+  </si>
+  <si>
+    <t>Late Sparks</t>
+  </si>
+  <si>
+    <t>Support_ID</t>
+  </si>
+  <si>
+    <t>End Sparks</t>
+  </si>
+  <si>
+    <t>varchar(100)</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>varchar(4)</t>
+  </si>
+  <si>
+    <t>default 'G'</t>
+  </si>
+  <si>
+    <t>support type</t>
   </si>
   <si>
     <t>varchar(7)</t>
   </si>
   <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>boolean</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
     <t>Rarity</t>
   </si>
   <si>
@@ -139,118 +244,19 @@
     <t>Limit Break</t>
   </si>
   <si>
-    <t>default 0</t>
-  </si>
-  <si>
-    <t>Speed Sparks</t>
-  </si>
-  <si>
-    <t>Deck</t>
-  </si>
-  <si>
-    <t>Stamina Sparks</t>
-  </si>
-  <si>
-    <t>Power Sparks</t>
-  </si>
-  <si>
-    <t>Support 1</t>
-  </si>
-  <si>
-    <t>Guts Sparks</t>
-  </si>
-  <si>
-    <t>Support 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">int </t>
-  </si>
-  <si>
-    <t>Wit Sparks</t>
-  </si>
-  <si>
-    <t>Support 3</t>
-  </si>
-  <si>
-    <t>Turf Sparks</t>
-  </si>
-  <si>
-    <t>Support 4</t>
-  </si>
-  <si>
-    <t>Dirt Sparks</t>
-  </si>
-  <si>
-    <t>Support 5</t>
-  </si>
-  <si>
-    <t>Sprint Sparks</t>
-  </si>
-  <si>
-    <t>Support 6</t>
-  </si>
-  <si>
-    <t>Mile Sparks</t>
-  </si>
-  <si>
-    <t>Medium Sparks</t>
-  </si>
-  <si>
-    <t>Long Sparks</t>
-  </si>
-  <si>
-    <t>Support Card</t>
-  </si>
-  <si>
-    <t>Front Sparks</t>
-  </si>
-  <si>
-    <t>Support_ID</t>
-  </si>
-  <si>
-    <t>Pace Sparks</t>
-  </si>
-  <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
-    <t>Late Sparks</t>
-  </si>
-  <si>
-    <t>support type</t>
-  </si>
-  <si>
-    <t>End Sparks</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>varchar(4)</t>
-  </si>
-  <si>
-    <t>default 'G'</t>
-  </si>
-  <si>
-    <t>tinyint</t>
-  </si>
-  <si>
-    <t>Completed</t>
-  </si>
-  <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>Run skills</t>
   </si>
   <si>
     <t>skill_id</t>
   </si>
   <si>
+    <t>Skills</t>
+  </si>
+  <si>
     <t>run_id</t>
+  </si>
+  <si>
+    <t>skill_name</t>
   </si>
 </sst>
 </file>
@@ -311,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,6 +364,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00FF"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
       </patternFill>
     </fill>
   </fills>
@@ -411,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -448,6 +460,9 @@
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -470,6 +485,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1040,7 +1058,7 @@
       <c r="E16" s="9"/>
       <c r="F16" s="9"/>
       <c r="H16" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I16" s="5" t="s">
         <v>26</v>
@@ -1054,7 +1072,7 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>26</v>
@@ -1066,7 +1084,7 @@
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
       <c r="H17" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>26</v>
@@ -1080,7 +1098,7 @@
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>26</v>
@@ -1092,7 +1110,7 @@
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
       <c r="H18" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>26</v>
@@ -1106,7 +1124,7 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>26</v>
@@ -1118,7 +1136,7 @@
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
       <c r="H19" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I19" s="5" t="s">
         <v>26</v>
@@ -1132,7 +1150,7 @@
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>26</v>
@@ -1144,7 +1162,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="H20" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>26</v>
@@ -1158,16 +1176,16 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="H21" s="5" t="s">
         <v>33</v>
@@ -1184,16 +1202,16 @@
     </row>
     <row r="22">
       <c r="A22" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+        <v>26</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="9"/>
       <c r="H22" s="5" t="s">
         <v>34</v>
@@ -1210,15 +1228,17 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>4</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="9"/>
       <c r="H23" s="5" t="s">
@@ -1235,8 +1255,13 @@
       <c r="M23" s="9"/>
     </row>
     <row r="24">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
       <c r="H24" s="5" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>3</v>
@@ -1245,22 +1270,19 @@
         <v>4</v>
       </c>
       <c r="K24" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L24" s="5"/>
       <c r="M24" s="9"/>
     </row>
     <row r="25">
-      <c r="A25" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
       <c r="H25" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I25" s="5" t="s">
         <v>3</v>
@@ -1269,32 +1291,14 @@
         <v>4</v>
       </c>
       <c r="K25" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L25" s="5"/>
       <c r="M25" s="9"/>
     </row>
     <row r="26">
-      <c r="A26" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>7</v>
-      </c>
       <c r="H26" s="5" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I26" s="5" t="s">
         <v>3</v>
@@ -1303,28 +1307,22 @@
         <v>4</v>
       </c>
       <c r="K26" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L26" s="5"/>
       <c r="M26" s="9"/>
     </row>
     <row r="27">
-      <c r="A27" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A27" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
       <c r="H27" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>3</v>
@@ -1333,28 +1331,32 @@
         <v>4</v>
       </c>
       <c r="K27" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L27" s="5"/>
       <c r="M27" s="9"/>
     </row>
     <row r="28">
       <c r="A28" s="5" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="15" t="s">
-        <v>14</v>
+      <c r="D28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="I28" s="5" t="s">
         <v>3</v>
@@ -1363,345 +1365,373 @@
         <v>4</v>
       </c>
       <c r="K28" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="L28" s="5"/>
       <c r="M28" s="9"/>
     </row>
     <row r="29">
       <c r="A29" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H29" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J29" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K29" s="16" t="s">
-        <v>42</v>
+      <c r="H29" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K29" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L29" s="5"/>
       <c r="M29" s="9"/>
     </row>
     <row r="30">
       <c r="A30" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="5"/>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H30" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J30" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K30" s="16" t="s">
-        <v>42</v>
+      <c r="H30" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="I30" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K30" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L30" s="5"/>
       <c r="M30" s="9"/>
     </row>
     <row r="31">
       <c r="A31" s="5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="5"/>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H31" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J31" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K31" s="16" t="s">
-        <v>42</v>
+      <c r="H31" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K31" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L31" s="5"/>
       <c r="M31" s="9"/>
     </row>
     <row r="32">
       <c r="A32" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="H32" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J32" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="16" t="s">
-        <v>42</v>
+      <c r="H32" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I32" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K32" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L32" s="5"/>
       <c r="M32" s="9"/>
     </row>
     <row r="33">
-      <c r="H33" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I33" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J33" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K33" s="16" t="s">
-        <v>42</v>
+      <c r="A33" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="I33" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K33" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L33" s="5"/>
       <c r="M33" s="9"/>
     </row>
     <row r="34">
-      <c r="H34" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>42</v>
+      <c r="A34" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J34" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L34" s="5"/>
       <c r="M34" s="9"/>
     </row>
     <row r="35">
-      <c r="A35" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3"/>
-      <c r="H35" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="I35" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J35" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K35" s="16" t="s">
-        <v>42</v>
+      <c r="H35" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="I35" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L35" s="5"/>
       <c r="M35" s="9"/>
     </row>
     <row r="36">
-      <c r="A36" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="I36" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J36" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K36" s="16" t="s">
-        <v>42</v>
+      <c r="H36" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J36" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K36" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L36" s="5"/>
       <c r="M36" s="9"/>
     </row>
     <row r="37">
-      <c r="A37" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="H37" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="I37" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J37" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K37" s="16" t="s">
-        <v>42</v>
+      <c r="A37" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="3"/>
+      <c r="H37" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L37" s="5"/>
       <c r="M37" s="9"/>
     </row>
     <row r="38">
       <c r="A38" s="5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>37</v>
+        <v>3</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="H38" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="I38" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="J38" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K38" s="16" t="s">
-        <v>42</v>
+      <c r="D38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J38" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>39</v>
       </c>
       <c r="L38" s="5"/>
       <c r="M38" s="9"/>
     </row>
     <row r="39">
       <c r="A39" s="5" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="H39" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="I39" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J39" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="K39" s="16" t="s">
-        <v>72</v>
+      <c r="H39" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="J39" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="L39" s="5"/>
       <c r="M39" s="9"/>
     </row>
     <row r="40">
       <c r="A40" s="5" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>42</v>
-      </c>
+      <c r="D40" s="9"/>
       <c r="E40" s="9"/>
       <c r="F40" s="9"/>
-      <c r="H40" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="I40" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="J40" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="K40" s="18" t="b">
+      <c r="H40" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="J40" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="K40" s="19" t="b">
         <v>0</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
     </row>
     <row r="41">
-      <c r="H41" s="19"/>
-      <c r="I41" s="19"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="A41" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
     </row>
     <row r="42">
-      <c r="H42" s="20" t="s">
+      <c r="A42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="H42" s="21" t="s">
         <v>77</v>
       </c>
       <c r="I42" s="2"/>
@@ -1718,13 +1748,21 @@
       <c r="J43" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K43" s="21" t="s">
+      <c r="K43" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="44">
+      <c r="A44" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="3"/>
       <c r="H44" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I44" s="5" t="s">
         <v>3</v>
@@ -1736,14 +1774,43 @@
         <v>14</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H42:K42"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A35:F35"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A44:F44"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>